<commit_message>
working on main function
</commit_message>
<xml_diff>
--- a/input/df_input.xlsx
+++ b/input/df_input.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\02. Mestrado\TU Darmstadt\Energy Science and Engineering\5. Sommersemester 2023\Masterarbeit\5. Thesis\3. Python Routine\masterthesis\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6A0E67-EFEF-41F3-A253-8BCF00D4CFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984FA8B3-5A4D-4C07-B5B0-49B3C52FCC08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="series" sheetId="1" r:id="rId1"/>
     <sheet name="other" sheetId="2" r:id="rId2"/>
     <sheet name="power_constraints" sheetId="3" r:id="rId3"/>
+    <sheet name="constraints" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">constraints!$A$9:$A$25</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
   <si>
     <t>HOURS</t>
   </si>
@@ -104,6 +108,69 @@
   </si>
   <si>
     <t>net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from </t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>pv_bat</t>
+  </si>
+  <si>
+    <t>pv_demand</t>
+  </si>
+  <si>
+    <t>pv_net</t>
+  </si>
+  <si>
+    <t>bat_pv</t>
+  </si>
+  <si>
+    <t>bat_net</t>
+  </si>
+  <si>
+    <t>demand_pv</t>
+  </si>
+  <si>
+    <t>demand_bat</t>
+  </si>
+  <si>
+    <t>net_pv</t>
+  </si>
+  <si>
+    <t>net_bat</t>
+  </si>
+  <si>
+    <t>net_demand</t>
+  </si>
+  <si>
+    <t>bat_demand</t>
+  </si>
+  <si>
+    <t>demand_net</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>gen -&gt; consumer</t>
+  </si>
+  <si>
+    <t>gen -&gt; storage</t>
+  </si>
+  <si>
+    <t>storage -&gt; consumer</t>
+  </si>
+  <si>
+    <t>storage -&gt; net</t>
+  </si>
+  <si>
+    <t>gen -&gt; net</t>
+  </si>
+  <si>
+    <t>Combinacao nao soh dos componentes, mas dos tipos que eles sao, e ai elimina os que nao fazem sentido.</t>
   </si>
 </sst>
 </file>
@@ -1076,8 +1143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65717FF-4051-4919-9693-46CD3A77ED5F}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1174,4 +1241,1068 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8FADEA-F7AF-4C95-A8C5-146429D458AF}">
+  <dimension ref="A1:Q32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="10.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.15625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.26171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.1015625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="6.1015625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.68359375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.7890625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.68359375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.1015625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.7890625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.68359375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="str">
+        <f>$A3&amp;"_"&amp;C$2</f>
+        <v>pv_bat</v>
+      </c>
+      <c r="D3" t="str">
+        <f>$A3&amp;"_"&amp;D$2</f>
+        <v>pv_demand</v>
+      </c>
+      <c r="E3" t="str">
+        <f>$A3&amp;"_"&amp;E$2</f>
+        <v>pv_net</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="str">
+        <f>$A4&amp;"_"&amp;B$2</f>
+        <v>bat_pv</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="str">
+        <f>$A4&amp;"_"&amp;D$2</f>
+        <v>bat_demand</v>
+      </c>
+      <c r="E4" t="str">
+        <f>$A4&amp;"_"&amp;E$2</f>
+        <v>bat_net</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="str">
+        <f>$A5&amp;"_"&amp;B$2</f>
+        <v>demand_pv</v>
+      </c>
+      <c r="C5" t="str">
+        <f>$A5&amp;"_"&amp;C$2</f>
+        <v>demand_bat</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="str">
+        <f>$A5&amp;"_"&amp;E$2</f>
+        <v>demand_net</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="str">
+        <f>$A6&amp;"_"&amp;B$2</f>
+        <v>net_pv</v>
+      </c>
+      <c r="C6" t="str">
+        <f>$A6&amp;"_"&amp;C$2</f>
+        <v>net_bat</v>
+      </c>
+      <c r="D6" t="str">
+        <f>$A6&amp;"_"&amp;D$2</f>
+        <v>net_demand</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" t="s">
+        <v>32</v>
+      </c>
+      <c r="L9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" t="s">
+        <v>34</v>
+      </c>
+      <c r="N9" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" t="s">
+        <v>26</v>
+      </c>
+      <c r="P9" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="D27" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="D28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="D29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="D31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="D32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A9:A25" xr:uid="{6B8FADEA-F7AF-4C95-A8C5-146429D458AF}"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Last version before starting connect
</commit_message>
<xml_diff>
--- a/input/df_input.xlsx
+++ b/input/df_input.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\02. Mestrado\TU Darmstadt\Energy Science and Engineering\5. Sommersemester 2023\Masterarbeit\5. Thesis\3. Python Routine\masterthesis\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930138BB-268E-4DB2-9D22-681A46B92196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95EA301B-0206-473C-BFDF-9F9FAD8E4102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="series" sheetId="1" r:id="rId1"/>
     <sheet name="other" sheetId="2" r:id="rId2"/>
-    <sheet name="elements" sheetId="5" r:id="rId3"/>
-    <sheet name="connect_to" sheetId="9" r:id="rId4"/>
-    <sheet name="connect_from" sheetId="10" r:id="rId5"/>
+    <sheet name="aux" sheetId="10" r:id="rId3"/>
+    <sheet name="elements" sheetId="5" r:id="rId4"/>
+    <sheet name="conect" sheetId="9" r:id="rId5"/>
     <sheet name="pv" sheetId="7" r:id="rId6"/>
     <sheet name="bat" sheetId="8" r:id="rId7"/>
     <sheet name="hyperclass" sheetId="6" r:id="rId8"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>HOURS</t>
   </si>
@@ -78,9 +78,6 @@
     <t>P_solar</t>
   </si>
   <si>
-    <t>P_demand</t>
-  </si>
-  <si>
     <t>starting_SOC</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>bat_dis_eff</t>
   </si>
   <si>
-    <t>e_to_q_ratio</t>
-  </si>
-  <si>
     <t>objective</t>
   </si>
   <si>
@@ -133,6 +127,21 @@
   </si>
   <si>
     <t>net</t>
+  </si>
+  <si>
+    <t>P_to_demand</t>
+  </si>
+  <si>
+    <t>PV</t>
+  </si>
+  <si>
+    <t>BAT</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>m</t>
   </si>
 </sst>
 </file>
@@ -462,7 +471,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F7" sqref="E7:F7"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -484,10 +493,10 @@
         <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1001,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8905AAD9-0A3E-4484-91AE-7843DE064B87}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B10"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1023,7 +1032,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>0.5</v>
@@ -1073,7 +1082,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>0.95</v>
@@ -1081,25 +1090,20 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>0.95</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="1"/>
-    </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="H19" s="1"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F16" s="1"/>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1108,21 +1112,50 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CAFF5BD-911A-46C0-BBEF-4997C72A1435}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD14CA6-CD17-4C1C-A259-2DC4938A6A0C}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1130,7 +1163,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1141,104 +1174,6 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E7" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{132E8599-A25F-4552-80A2-9C4B08641A54}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1247,96 +1182,102 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{616600D1-84E9-4C66-841D-878B041D9339}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{132E8599-A25F-4552-80A2-9C4B08641A54}">
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="B2:E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>28</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
         <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="I7" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="H10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1349,14 +1290,14 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -1375,7 +1316,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1392,10 +1333,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9D187A-0F4F-41A2-AA05-09A6BD6BC1F5}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1403,36 +1344,20 @@
     <col min="1" max="1" width="3.7890625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.83984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.47265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1015625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.41796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.47265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1440,19 +1365,7 @@
         <v>0.5</v>
       </c>
       <c r="C2">
-        <v>100</v>
-      </c>
-      <c r="D2">
-        <v>0.95</v>
-      </c>
-      <c r="E2">
-        <v>0.95</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -1465,8 +1378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C169D9-10BE-4807-B445-94CDCC7FA162}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1484,34 +1397,34 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
I am going to branch this
</commit_message>
<xml_diff>
--- a/input/df_input.xlsx
+++ b/input/df_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\02. Mestrado\TU Darmstadt\Energy Science and Engineering\5. Sommersemester 2023\Masterarbeit\5. Thesis\3. Python Routine\masterthesis\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95EA301B-0206-473C-BFDF-9F9FAD8E4102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C384463-C67D-4140-8F90-DDB8C86E0F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="series" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>HOURS</t>
   </si>
@@ -1013,7 +1013,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1113,10 +1113,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CAFF5BD-911A-46C0-BBEF-4997C72A1435}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1135,6 +1135,14 @@
       </c>
       <c r="B2" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1146,7 +1154,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD14CA6-CD17-4C1C-A259-2DC4938A6A0C}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
@@ -1186,7 +1196,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1289,8 +1299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DEA67B-B7E8-4C04-ABA0-043F84E9EB2D}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1308,15 +1318,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1336,7 +1338,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1378,8 +1380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C169D9-10BE-4807-B445-94CDCC7FA162}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
ups i did it again
</commit_message>
<xml_diff>
--- a/input/df_input.xlsx
+++ b/input/df_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\02. Mestrado\TU Darmstadt\Energy Science and Engineering\5. Sommersemester 2023\Masterarbeit\5. Thesis\3. Python Routine\masterthesis\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72DA029-FAF7-4650-B4DF-367A0CBA6AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BC130C-B4ED-4781-83B5-32B77E4C9B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="series" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>HOURS</t>
   </si>
@@ -123,9 +123,6 @@
     <t>net</t>
   </si>
   <si>
-    <t>P_to_demand</t>
-  </si>
-  <si>
     <t>PV</t>
   </si>
   <si>
@@ -151,6 +148,15 @@
   </si>
   <si>
     <t>bat1</t>
+  </si>
+  <si>
+    <t>P_to_demand1</t>
+  </si>
+  <si>
+    <t>E_bat1_max</t>
+  </si>
+  <si>
+    <t>pv1_eff</t>
   </si>
 </sst>
 </file>
@@ -506,7 +512,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -528,7 +534,7 @@
         <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s">
         <v>12</v>
@@ -1047,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8905AAD9-0A3E-4484-91AE-7843DE064B87}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1075,7 +1081,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="B3">
         <v>100</v>
@@ -1083,7 +1089,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="B4">
         <v>0.5</v>
@@ -1166,18 +1172,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
         <v>29</v>
-      </c>
-      <c r="B2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
         <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1189,9 +1195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD14CA6-CD17-4C1C-A259-2DC4938A6A0C}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
@@ -1250,24 +1254,24 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1287,7 +1291,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1307,7 +1311,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1327,7 +1331,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1347,7 +1351,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1389,7 +1393,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -1432,7 +1436,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
dynamically creating connection constraints
</commit_message>
<xml_diff>
--- a/input/df_input.xlsx
+++ b/input/df_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\02. Mestrado\TU Darmstadt\Energy Science and Engineering\5. Sommersemester 2023\Masterarbeit\5. Thesis\3. Python Routine\masterthesis\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BC130C-B4ED-4781-83B5-32B77E4C9B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A494660-0B1F-4D6A-9559-E34C91E9F5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="series" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>HOURS</t>
   </si>
@@ -142,9 +142,6 @@
   </si>
   <si>
     <t>pv1</t>
-  </si>
-  <si>
-    <t>pv2</t>
   </si>
   <si>
     <t>bat1</t>
@@ -223,12 +220,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,7 +532,7 @@
         <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
         <v>12</v>
@@ -1053,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8905AAD9-0A3E-4484-91AE-7843DE064B87}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1081,7 +1079,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>100</v>
@@ -1089,7 +1087,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>0.5</v>
@@ -1244,15 +1242,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{132E8599-A25F-4552-80A2-9C4B08641A54}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1265,11 +1263,8 @@
       <c r="E1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
@@ -1285,11 +1280,8 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -1305,18 +1297,15 @@
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>0</v>
       </c>
       <c r="D4">
@@ -1325,11 +1314,8 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -1337,43 +1323,14 @@
         <v>0</v>
       </c>
       <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
         <v>0</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="I7" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="H10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
flexible working with classes!
</commit_message>
<xml_diff>
--- a/input/df_input.xlsx
+++ b/input/df_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\02. Mestrado\TU Darmstadt\Energy Science and Engineering\5. Sommersemester 2023\Masterarbeit\5. Thesis\3. Python Routine\masterthesis\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175D0942-3F23-4B30-9706-FDC586DAE922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC5CD80-98BE-4B52-98FB-FE231A034120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Parameter</t>
   </si>
@@ -69,6 +69,30 @@
   </si>
   <si>
     <t>bat1_dis_eff</t>
+  </si>
+  <si>
+    <t>pv2_eff</t>
+  </si>
+  <si>
+    <t>pv2_area</t>
+  </si>
+  <si>
+    <t>bat2_c_rate_ch</t>
+  </si>
+  <si>
+    <t>bat2_c_rate_dis</t>
+  </si>
+  <si>
+    <t>bat2_ch_eff</t>
+  </si>
+  <si>
+    <t>bat2_dis_eff</t>
+  </si>
+  <si>
+    <t>bat2_starting_SOC</t>
+  </si>
+  <si>
+    <t>bat2_E_max</t>
   </si>
   <si>
     <t>HOURS</t>
@@ -457,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -482,7 +506,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -490,7 +514,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -549,6 +573,70 @@
       </c>
       <c r="B10">
         <v>0.95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -562,26 +650,26 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1017,32 +1105,35 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1055,9 +1146,13 @@
       <c r="D2">
         <v>1</v>
       </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -1073,21 +1168,21 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1104,7 +1199,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1121,7 +1216,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1138,7 +1233,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B5">
         <v>0</v>

</xml_diff>

<commit_message>
first attempt with automatic reading
</commit_message>
<xml_diff>
--- a/input/df_input.xlsx
+++ b/input/df_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\02. Mestrado\TU Darmstadt\Energy Science and Engineering\5. Sommersemester 2023\Masterarbeit\5. Thesis\3. Python Routine\masterthesis\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAC1689-A146-4160-B198-89484D7139E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F040BF0F-7DF8-4519-8020-51849877A168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="other" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Parameter</t>
   </si>
@@ -50,12 +50,6 @@
     <t>bat1_E_max</t>
   </si>
   <si>
-    <t>pv1_eff</t>
-  </si>
-  <si>
-    <t>pv1_area</t>
-  </si>
-  <si>
     <t>time_step</t>
   </si>
   <si>
@@ -134,13 +128,7 @@
     <t>demand1</t>
   </si>
   <si>
-    <t>demand2</t>
-  </si>
-  <si>
     <t>net1</t>
-  </si>
-  <si>
-    <t>net2</t>
   </si>
   <si>
     <t>pv1</t>
@@ -496,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G4:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -537,7 +525,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -547,6 +535,7 @@
       <c r="B5">
         <v>1</v>
       </c>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
@@ -555,31 +544,30 @@
       <c r="B6">
         <v>1</v>
       </c>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1"/>
+        <v>0.95</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1"/>
+        <v>0.95</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.95</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -587,7 +575,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -595,7 +583,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -611,7 +599,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -619,7 +607,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -627,7 +615,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>0.95</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -635,22 +623,6 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18">
         <v>200</v>
       </c>
     </row>
@@ -665,7 +637,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -680,28 +652,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>24</v>
-      </c>
-      <c r="G1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1362,31 +1334,31 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1406,60 +1378,48 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1471,18 +1431,12 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1496,79 +1450,21 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatic reading works fine
</commit_message>
<xml_diff>
--- a/input/df_input.xlsx
+++ b/input/df_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\02. Mestrado\TU Darmstadt\Energy Science and Engineering\5. Sommersemester 2023\Masterarbeit\5. Thesis\3. Python Routine\masterthesis\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F040BF0F-7DF8-4519-8020-51849877A168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0AB686-F41A-4DE3-AB6D-232EE14F5D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="other" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Parameter</t>
   </si>
@@ -44,27 +44,9 @@
     <t>Value</t>
   </si>
   <si>
-    <t>bat1_starting_SOC</t>
-  </si>
-  <si>
-    <t>bat1_E_max</t>
-  </si>
-  <si>
     <t>time_step</t>
   </si>
   <si>
-    <t>bat1_c_rate_ch</t>
-  </si>
-  <si>
-    <t>bat1_c_rate_dis</t>
-  </si>
-  <si>
-    <t>bat1_ch_eff</t>
-  </si>
-  <si>
-    <t>bat1_dis_eff</t>
-  </si>
-  <si>
     <t>pv2_eff</t>
   </si>
   <si>
@@ -92,49 +74,49 @@
     <t>HOURS</t>
   </si>
   <si>
+    <t>net2_cost_buy</t>
+  </si>
+  <si>
+    <t>net2_cost_sell</t>
+  </si>
+  <si>
+    <t>P_to_demand1</t>
+  </si>
+  <si>
+    <t>P_solar</t>
+  </si>
+  <si>
+    <t>demand</t>
+  </si>
+  <si>
+    <t>net</t>
+  </si>
+  <si>
+    <t>pv</t>
+  </si>
+  <si>
+    <t>bat</t>
+  </si>
+  <si>
+    <t>demand1</t>
+  </si>
+  <si>
+    <t>net1</t>
+  </si>
+  <si>
+    <t>pv1</t>
+  </si>
+  <si>
+    <t>bat1</t>
+  </si>
+  <si>
+    <t>net1_cost_sell</t>
+  </si>
+  <si>
     <t>net1_cost_buy</t>
   </si>
   <si>
-    <t>net1_cost_sell</t>
-  </si>
-  <si>
-    <t>net2_cost_buy</t>
-  </si>
-  <si>
-    <t>net2_cost_sell</t>
-  </si>
-  <si>
-    <t>P_solar</t>
-  </si>
-  <si>
-    <t>P_to_demand1</t>
-  </si>
-  <si>
-    <t>P_to_demand2</t>
-  </si>
-  <si>
-    <t>demand</t>
-  </si>
-  <si>
-    <t>net</t>
-  </si>
-  <si>
-    <t>pv</t>
-  </si>
-  <si>
-    <t>bat</t>
-  </si>
-  <si>
-    <t>demand1</t>
-  </si>
-  <si>
-    <t>net1</t>
-  </si>
-  <si>
-    <t>pv1</t>
-  </si>
-  <si>
-    <t>bat1</t>
+    <t>Q_to_demand1</t>
   </si>
 </sst>
 </file>
@@ -198,12 +180,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G4:G5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -496,7 +480,7 @@
     <col min="2" max="2" width="5.1015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -504,23 +488,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -528,25 +512,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -554,7 +536,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -562,67 +544,19 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
         <v>200</v>
       </c>
     </row>
@@ -634,450 +568,467 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B1" sqref="B1:H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="6.41796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.9453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.9453125" customWidth="1"/>
-    <col min="6" max="6" width="6.47265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1015625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7890625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.9453125" customWidth="1"/>
+    <col min="5" max="6" width="12.3125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.9453125" customWidth="1"/>
+    <col min="8" max="8" width="6.47265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.47</v>
+        <f ca="1">RANDBETWEEN(700,1000)</f>
+        <v>878</v>
       </c>
       <c r="C2">
-        <v>0.31</v>
+        <v>428</v>
       </c>
       <c r="D2">
-        <v>0.48</v>
+        <v>0.42</v>
       </c>
       <c r="E2">
         <v>0.4</v>
       </c>
       <c r="F2">
+        <v>0.48</v>
+      </c>
+      <c r="G2">
+        <v>0.33</v>
+      </c>
+      <c r="H2">
         <v>893</v>
       </c>
-      <c r="G2">
-        <v>485</v>
-      </c>
-      <c r="H2">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <f t="shared" ref="A3:A25" si="0">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3">
+        <f t="shared" ref="B3:B25" ca="1" si="1">RANDBETWEEN(700,1000)</f>
+        <v>797</v>
+      </c>
+      <c r="C3">
+        <v>431</v>
+      </c>
+      <c r="D3">
         <v>0.46</v>
-      </c>
-      <c r="C3">
-        <v>0.3</v>
-      </c>
-      <c r="D3">
-        <v>0.4</v>
       </c>
       <c r="E3">
         <v>0.38</v>
       </c>
       <c r="F3">
+        <v>0.4</v>
+      </c>
+      <c r="G3">
+        <v>0.39</v>
+      </c>
+      <c r="H3">
         <v>632</v>
       </c>
-      <c r="G3">
-        <v>444</v>
-      </c>
-      <c r="H3">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.5</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>861</v>
       </c>
       <c r="C4">
-        <v>0.36</v>
+        <v>491</v>
       </c>
       <c r="D4">
-        <v>0.49</v>
+        <v>0.4</v>
       </c>
       <c r="E4">
         <v>0.3</v>
       </c>
       <c r="F4">
+        <v>0.49</v>
+      </c>
+      <c r="G4">
+        <v>0.38</v>
+      </c>
+      <c r="H4">
         <v>212</v>
       </c>
-      <c r="G4">
-        <v>384</v>
-      </c>
-      <c r="H4">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.44</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>882</v>
       </c>
       <c r="C5">
-        <v>0.32</v>
+        <v>316</v>
       </c>
       <c r="D5">
-        <v>0.43</v>
+        <v>0.45</v>
       </c>
       <c r="E5">
         <v>0.34</v>
       </c>
       <c r="F5">
+        <v>0.43</v>
+      </c>
+      <c r="G5">
+        <v>0.35</v>
+      </c>
+      <c r="H5">
         <v>580</v>
       </c>
-      <c r="G5">
-        <v>325</v>
-      </c>
-      <c r="H5">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.47</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>706</v>
       </c>
       <c r="C6">
-        <v>0.32</v>
+        <v>491</v>
       </c>
       <c r="D6">
-        <v>0.47</v>
+        <v>0.41</v>
       </c>
       <c r="E6">
         <v>0.31</v>
       </c>
       <c r="F6">
+        <v>0.47</v>
+      </c>
+      <c r="G6">
+        <v>0.37</v>
+      </c>
+      <c r="H6">
         <v>607</v>
       </c>
-      <c r="G6">
-        <v>394</v>
-      </c>
-      <c r="H6">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.41</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>833</v>
       </c>
       <c r="C7">
-        <v>0.37</v>
+        <v>328</v>
       </c>
       <c r="D7">
-        <v>0.49</v>
+        <v>0.48</v>
       </c>
       <c r="E7">
         <v>0.36</v>
       </c>
       <c r="F7">
+        <v>0.49</v>
+      </c>
+      <c r="G7">
+        <v>0.38</v>
+      </c>
+      <c r="H7">
         <v>177</v>
       </c>
-      <c r="G7">
-        <v>436</v>
-      </c>
-      <c r="H7">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.45</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>877</v>
       </c>
       <c r="C8">
-        <v>0.3</v>
+        <v>320</v>
       </c>
       <c r="D8">
-        <v>0.44</v>
+        <v>0.46</v>
       </c>
       <c r="E8">
         <v>0.38</v>
       </c>
       <c r="F8">
+        <v>0.44</v>
+      </c>
+      <c r="G8">
+        <v>0.3</v>
+      </c>
+      <c r="H8">
         <v>735</v>
       </c>
-      <c r="G8">
-        <v>423</v>
-      </c>
-      <c r="H8">
-        <v>946</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.4</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>731</v>
       </c>
       <c r="C9">
-        <v>0.36</v>
+        <v>463</v>
       </c>
       <c r="D9">
-        <v>0.48</v>
+        <v>0.47</v>
       </c>
       <c r="E9">
         <v>0.39</v>
       </c>
       <c r="F9">
+        <v>0.48</v>
+      </c>
+      <c r="G9">
+        <v>0.37</v>
+      </c>
+      <c r="H9">
         <v>879</v>
       </c>
-      <c r="G9">
-        <v>459</v>
-      </c>
-      <c r="H9">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0.46</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>882</v>
       </c>
       <c r="C10">
-        <v>0.34</v>
+        <v>444</v>
       </c>
       <c r="D10">
-        <v>0.48</v>
+        <v>0.4</v>
       </c>
       <c r="E10">
         <v>0.35</v>
       </c>
       <c r="F10">
+        <v>0.48</v>
+      </c>
+      <c r="G10">
+        <v>0.39</v>
+      </c>
+      <c r="H10">
         <v>731</v>
       </c>
-      <c r="G10">
-        <v>406</v>
-      </c>
-      <c r="H10">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0.4</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>750</v>
       </c>
       <c r="C11">
-        <v>0.33</v>
+        <v>473</v>
       </c>
       <c r="D11">
-        <v>0.41</v>
+        <v>0.44</v>
       </c>
       <c r="E11">
         <v>0.34</v>
       </c>
       <c r="F11">
+        <v>0.41</v>
+      </c>
+      <c r="G11">
+        <v>0.31</v>
+      </c>
+      <c r="H11">
         <v>281</v>
       </c>
-      <c r="G11">
-        <v>300</v>
-      </c>
-      <c r="H11">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0.4</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>894</v>
       </c>
       <c r="C12">
-        <v>0.4</v>
+        <v>329</v>
       </c>
       <c r="D12">
-        <v>0.44</v>
+        <v>0.43</v>
       </c>
       <c r="E12">
         <v>0.38</v>
       </c>
       <c r="F12">
+        <v>0.44</v>
+      </c>
+      <c r="G12">
+        <v>0.31</v>
+      </c>
+      <c r="H12">
         <v>232</v>
       </c>
-      <c r="G12">
-        <v>435</v>
-      </c>
-      <c r="H12">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0.46</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>772</v>
       </c>
       <c r="C13">
-        <v>0.36</v>
+        <v>418</v>
       </c>
       <c r="D13">
-        <v>0.47</v>
+        <v>0.41</v>
       </c>
       <c r="E13">
         <v>0.39</v>
       </c>
       <c r="F13">
+        <v>0.47</v>
+      </c>
+      <c r="G13">
+        <v>0.4</v>
+      </c>
+      <c r="H13">
         <v>390</v>
       </c>
-      <c r="G13">
-        <v>470</v>
-      </c>
-      <c r="H13">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.43</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>811</v>
       </c>
       <c r="C14">
-        <v>0.32</v>
+        <v>496</v>
       </c>
       <c r="D14">
-        <v>0.42</v>
+        <v>0.48</v>
       </c>
       <c r="E14">
         <v>0.33</v>
       </c>
       <c r="F14">
+        <v>0.42</v>
+      </c>
+      <c r="G14">
+        <v>0.34</v>
+      </c>
+      <c r="H14">
         <v>883</v>
       </c>
-      <c r="G14">
-        <v>343</v>
-      </c>
-      <c r="H14">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.4</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>801</v>
       </c>
       <c r="C15">
-        <v>0.39</v>
+        <v>355</v>
       </c>
       <c r="D15">
-        <v>0.43</v>
+        <v>0.49</v>
       </c>
       <c r="E15">
         <v>0.34</v>
       </c>
       <c r="F15">
+        <v>0.43</v>
+      </c>
+      <c r="G15">
+        <v>0.32</v>
+      </c>
+      <c r="H15">
         <v>955</v>
       </c>
-      <c r="G15">
-        <v>485</v>
-      </c>
-      <c r="H15">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0.43</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>816</v>
       </c>
       <c r="C16">
-        <v>0.4</v>
+        <v>327</v>
       </c>
       <c r="D16">
-        <v>0.4</v>
+        <v>0.47</v>
       </c>
       <c r="E16">
         <v>0.32</v>
       </c>
       <c r="F16">
+        <v>0.4</v>
+      </c>
+      <c r="G16">
+        <v>0.4</v>
+      </c>
+      <c r="H16">
         <v>841</v>
-      </c>
-      <c r="G16">
-        <v>370</v>
-      </c>
-      <c r="H16">
-        <v>800</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1086,25 +1037,26 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.45</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>758</v>
       </c>
       <c r="C17">
-        <v>0.3</v>
+        <v>379</v>
       </c>
       <c r="D17">
-        <v>0.43</v>
+        <v>0.48</v>
       </c>
       <c r="E17">
         <v>0.39</v>
       </c>
       <c r="F17">
+        <v>0.43</v>
+      </c>
+      <c r="G17">
+        <v>0.32</v>
+      </c>
+      <c r="H17">
         <v>385</v>
-      </c>
-      <c r="G17">
-        <v>381</v>
-      </c>
-      <c r="H17">
-        <v>292</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1113,25 +1065,26 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0.41</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>994</v>
       </c>
       <c r="C18">
-        <v>0.38</v>
+        <v>440</v>
       </c>
       <c r="D18">
-        <v>0.41</v>
+        <v>0.49</v>
       </c>
       <c r="E18">
         <v>0.33</v>
       </c>
       <c r="F18">
+        <v>0.41</v>
+      </c>
+      <c r="G18">
+        <v>0.3</v>
+      </c>
+      <c r="H18">
         <v>672</v>
-      </c>
-      <c r="G18">
-        <v>397</v>
-      </c>
-      <c r="H18">
-        <v>717</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1140,25 +1093,26 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0.49</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>945</v>
       </c>
       <c r="C19">
-        <v>0.33</v>
+        <v>352</v>
       </c>
       <c r="D19">
-        <v>0.48</v>
+        <v>0.5</v>
       </c>
       <c r="E19">
         <v>0.31</v>
       </c>
       <c r="F19">
+        <v>0.48</v>
+      </c>
+      <c r="G19">
+        <v>0.36</v>
+      </c>
+      <c r="H19">
         <v>547</v>
-      </c>
-      <c r="G19">
-        <v>363</v>
-      </c>
-      <c r="H19">
-        <v>410</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1167,25 +1121,26 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0.41</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>806</v>
       </c>
       <c r="C20">
-        <v>0.38</v>
+        <v>381</v>
       </c>
       <c r="D20">
-        <v>0.46</v>
+        <v>0.47</v>
       </c>
       <c r="E20">
         <v>0.32</v>
       </c>
       <c r="F20">
+        <v>0.46</v>
+      </c>
+      <c r="G20">
+        <v>0.3</v>
+      </c>
+      <c r="H20">
         <v>552</v>
-      </c>
-      <c r="G20">
-        <v>436</v>
-      </c>
-      <c r="H20">
-        <v>606</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1194,25 +1149,26 @@
         <v>20</v>
       </c>
       <c r="B21">
+        <f t="shared" ca="1" si="1"/>
+        <v>838</v>
+      </c>
+      <c r="C21">
+        <v>354</v>
+      </c>
+      <c r="D21">
         <v>0.4</v>
-      </c>
-      <c r="C21">
-        <v>0.39</v>
-      </c>
-      <c r="D21">
-        <v>0.46</v>
       </c>
       <c r="E21">
         <v>0.31</v>
       </c>
       <c r="F21">
+        <v>0.46</v>
+      </c>
+      <c r="G21">
+        <v>0.31</v>
+      </c>
+      <c r="H21">
         <v>976</v>
-      </c>
-      <c r="G21">
-        <v>484</v>
-      </c>
-      <c r="H21">
-        <v>603</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1221,25 +1177,26 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>0.41</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>779</v>
       </c>
       <c r="C22">
-        <v>0.36</v>
+        <v>440</v>
       </c>
       <c r="D22">
-        <v>0.43</v>
+        <v>0.49</v>
       </c>
       <c r="E22">
         <v>0.3</v>
       </c>
       <c r="F22">
+        <v>0.43</v>
+      </c>
+      <c r="G22">
+        <v>0.34</v>
+      </c>
+      <c r="H22">
         <v>734</v>
-      </c>
-      <c r="G22">
-        <v>302</v>
-      </c>
-      <c r="H22">
-        <v>870</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1248,25 +1205,26 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>0.46</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>898</v>
       </c>
       <c r="C23">
-        <v>0.33</v>
+        <v>363</v>
       </c>
       <c r="D23">
-        <v>0.47</v>
+        <v>0.41</v>
       </c>
       <c r="E23">
         <v>0.39</v>
       </c>
       <c r="F23">
+        <v>0.47</v>
+      </c>
+      <c r="G23">
+        <v>0.39</v>
+      </c>
+      <c r="H23">
         <v>388</v>
-      </c>
-      <c r="G23">
-        <v>350</v>
-      </c>
-      <c r="H23">
-        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1275,10 +1233,11 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>0.48</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>994</v>
       </c>
       <c r="C24">
-        <v>0.39</v>
+        <v>397</v>
       </c>
       <c r="D24">
         <v>0.45</v>
@@ -1287,13 +1246,13 @@
         <v>0.4</v>
       </c>
       <c r="F24">
+        <v>0.45</v>
+      </c>
+      <c r="G24">
+        <v>0.4</v>
+      </c>
+      <c r="H24">
         <v>731</v>
-      </c>
-      <c r="G24">
-        <v>457</v>
-      </c>
-      <c r="H24">
-        <v>852</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1302,30 +1261,31 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>0.5</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>739</v>
       </c>
       <c r="C25">
-        <v>0.35</v>
+        <v>471</v>
       </c>
       <c r="D25">
-        <v>0.49</v>
+        <v>0.45</v>
       </c>
       <c r="E25">
         <v>0.4</v>
       </c>
       <c r="F25">
+        <v>0.49</v>
+      </c>
+      <c r="G25">
+        <v>0.36</v>
+      </c>
+      <c r="H25">
         <v>754</v>
-      </c>
-      <c r="G25">
-        <v>439</v>
-      </c>
-      <c r="H25">
-        <v>228</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1333,24 +1293,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1381,28 +1339,28 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:D5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>32</v>
+      <c r="B1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="2" t="s">
-        <v>29</v>
+      <c r="A2" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1418,8 +1376,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="2" t="s">
-        <v>30</v>
+      <c r="A3" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1435,8 +1393,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="2" t="s">
-        <v>31</v>
+      <c r="A4" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1452,8 +1410,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="2" t="s">
-        <v>32</v>
+      <c r="A5" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B5">
         <v>0</v>

</xml_diff>

<commit_message>
worked with heat demand
</commit_message>
<xml_diff>
--- a/input/df_input.xlsx
+++ b/input/df_input.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\02. Mestrado\TU Darmstadt\Energy Science and Engineering\5. Sommersemester 2023\Masterarbeit\5. Thesis\3. Python Routine\masterthesis\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0AB686-F41A-4DE3-AB6D-232EE14F5D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015E7023-980E-43DF-B8AA-E6D21C2828A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="other" sheetId="1" r:id="rId1"/>
     <sheet name="series" sheetId="2" r:id="rId2"/>
     <sheet name="elements" sheetId="3" r:id="rId3"/>
-    <sheet name="conect" sheetId="4" r:id="rId4"/>
+    <sheet name="elements test" sheetId="4" r:id="rId4"/>
+    <sheet name="conect_electric" sheetId="5" r:id="rId5"/>
+    <sheet name="conect_thermal" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>Parameter</t>
   </si>
@@ -74,18 +76,27 @@
     <t>HOURS</t>
   </si>
   <si>
-    <t>net2_cost_buy</t>
-  </si>
-  <si>
-    <t>net2_cost_sell</t>
+    <t>Q_to_demand1</t>
   </si>
   <si>
     <t>P_to_demand1</t>
   </si>
   <si>
+    <t>net1_cost_sell_electric</t>
+  </si>
+  <si>
+    <t>net1_cost_buy_electric</t>
+  </si>
+  <si>
     <t>P_solar</t>
   </si>
   <si>
+    <t>net1_cost_sell_thermal</t>
+  </si>
+  <si>
+    <t>net1_cost_buy_thermal</t>
+  </si>
+  <si>
     <t>demand</t>
   </si>
   <si>
@@ -98,6 +109,15 @@
     <t>bat</t>
   </si>
   <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t># components</t>
+  </si>
+  <si>
+    <t>CHP</t>
+  </si>
+  <si>
     <t>demand1</t>
   </si>
   <si>
@@ -110,20 +130,14 @@
     <t>bat1</t>
   </si>
   <si>
-    <t>net1_cost_sell</t>
-  </si>
-  <si>
-    <t>net1_cost_buy</t>
-  </si>
-  <si>
-    <t>Q_to_demand1</t>
+    <t>CHP1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +147,13 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -177,20 +198,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -568,10 +591,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -579,456 +602,441 @@
     <col min="1" max="1" width="6.41796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.1015625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7890625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.9453125" customWidth="1"/>
-    <col min="5" max="6" width="12.3125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.9453125" customWidth="1"/>
-    <col min="8" max="8" width="6.47265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1015625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.47265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.20703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>26</v>
+      <c r="B1" t="s">
+        <v>12</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
-        <v>24</v>
-      </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <f ca="1">RANDBETWEEN(700,1000)</f>
-        <v>878</v>
+        <v>984</v>
       </c>
       <c r="C2">
         <v>428</v>
       </c>
       <c r="D2">
+        <v>0.4</v>
+      </c>
+      <c r="E2">
         <v>0.42</v>
       </c>
-      <c r="E2">
+      <c r="F2">
+        <v>893</v>
+      </c>
+      <c r="G2">
+        <v>0.23</v>
+      </c>
+      <c r="H2">
         <v>0.4</v>
       </c>
-      <c r="F2">
-        <v>0.48</v>
-      </c>
-      <c r="G2">
-        <v>0.33</v>
-      </c>
-      <c r="H2">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <f t="shared" ref="A3:A25" si="0">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B25" ca="1" si="1">RANDBETWEEN(700,1000)</f>
-        <v>797</v>
+        <v>911</v>
       </c>
       <c r="C3">
         <v>431</v>
       </c>
       <c r="D3">
+        <v>0.38</v>
+      </c>
+      <c r="E3">
         <v>0.46</v>
       </c>
-      <c r="E3">
+      <c r="F3">
+        <v>632</v>
+      </c>
+      <c r="G3">
+        <v>0.25</v>
+      </c>
+      <c r="H3">
         <v>0.38</v>
       </c>
-      <c r="F3">
-        <v>0.4</v>
-      </c>
-      <c r="G3">
-        <v>0.39</v>
-      </c>
-      <c r="H3">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4">
-        <f t="shared" ca="1" si="1"/>
-        <v>861</v>
+        <v>873</v>
       </c>
       <c r="C4">
         <v>491</v>
       </c>
       <c r="D4">
+        <v>0.3</v>
+      </c>
+      <c r="E4">
         <v>0.4</v>
       </c>
-      <c r="E4">
+      <c r="F4">
+        <v>212</v>
+      </c>
+      <c r="G4">
+        <v>0.24</v>
+      </c>
+      <c r="H4">
         <v>0.3</v>
       </c>
-      <c r="F4">
-        <v>0.49</v>
-      </c>
-      <c r="G4">
-        <v>0.38</v>
-      </c>
-      <c r="H4">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5">
-        <f t="shared" ca="1" si="1"/>
-        <v>882</v>
+        <v>955</v>
       </c>
       <c r="C5">
         <v>316</v>
       </c>
       <c r="D5">
+        <v>0.34</v>
+      </c>
+      <c r="E5">
         <v>0.45</v>
       </c>
-      <c r="E5">
+      <c r="F5">
+        <v>580</v>
+      </c>
+      <c r="G5">
+        <v>0.2</v>
+      </c>
+      <c r="H5">
         <v>0.34</v>
       </c>
-      <c r="F5">
-        <v>0.43</v>
-      </c>
-      <c r="G5">
-        <v>0.35</v>
-      </c>
-      <c r="H5">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6">
-        <f t="shared" ca="1" si="1"/>
-        <v>706</v>
+        <v>736</v>
       </c>
       <c r="C6">
         <v>491</v>
       </c>
       <c r="D6">
+        <v>0.31</v>
+      </c>
+      <c r="E6">
         <v>0.41</v>
       </c>
-      <c r="E6">
+      <c r="F6">
+        <v>607</v>
+      </c>
+      <c r="G6">
+        <v>0.2</v>
+      </c>
+      <c r="H6">
         <v>0.31</v>
       </c>
-      <c r="F6">
-        <v>0.47</v>
-      </c>
-      <c r="G6">
-        <v>0.37</v>
-      </c>
-      <c r="H6">
-        <v>607</v>
-      </c>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7">
-        <f t="shared" ca="1" si="1"/>
-        <v>833</v>
+        <v>804</v>
       </c>
       <c r="C7">
         <v>328</v>
       </c>
       <c r="D7">
+        <v>0.36</v>
+      </c>
+      <c r="E7">
         <v>0.48</v>
       </c>
-      <c r="E7">
+      <c r="F7">
+        <v>177</v>
+      </c>
+      <c r="G7">
+        <v>0.22</v>
+      </c>
+      <c r="H7">
         <v>0.36</v>
       </c>
-      <c r="F7">
-        <v>0.49</v>
-      </c>
-      <c r="G7">
-        <v>0.38</v>
-      </c>
-      <c r="H7">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8">
-        <f t="shared" ca="1" si="1"/>
-        <v>877</v>
+        <v>726</v>
       </c>
       <c r="C8">
         <v>320</v>
       </c>
       <c r="D8">
+        <v>0.38</v>
+      </c>
+      <c r="E8">
         <v>0.46</v>
       </c>
-      <c r="E8">
+      <c r="F8">
+        <v>735</v>
+      </c>
+      <c r="G8">
+        <v>0.27</v>
+      </c>
+      <c r="H8">
         <v>0.38</v>
       </c>
-      <c r="F8">
-        <v>0.44</v>
-      </c>
-      <c r="G8">
-        <v>0.3</v>
-      </c>
-      <c r="H8">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9">
-        <f t="shared" ca="1" si="1"/>
-        <v>731</v>
+        <v>874</v>
       </c>
       <c r="C9">
         <v>463</v>
       </c>
       <c r="D9">
+        <v>0.39</v>
+      </c>
+      <c r="E9">
         <v>0.47</v>
       </c>
-      <c r="E9">
+      <c r="F9">
+        <v>879</v>
+      </c>
+      <c r="G9">
+        <v>0.27</v>
+      </c>
+      <c r="H9">
         <v>0.39</v>
       </c>
-      <c r="F9">
-        <v>0.48</v>
-      </c>
-      <c r="G9">
-        <v>0.37</v>
-      </c>
-      <c r="H9">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10">
-        <f t="shared" ca="1" si="1"/>
-        <v>882</v>
+        <v>853</v>
       </c>
       <c r="C10">
         <v>444</v>
       </c>
       <c r="D10">
+        <v>0.35</v>
+      </c>
+      <c r="E10">
         <v>0.4</v>
       </c>
-      <c r="E10">
+      <c r="F10">
+        <v>731</v>
+      </c>
+      <c r="G10">
+        <v>0.3</v>
+      </c>
+      <c r="H10">
         <v>0.35</v>
       </c>
-      <c r="F10">
-        <v>0.48</v>
-      </c>
-      <c r="G10">
-        <v>0.39</v>
-      </c>
-      <c r="H10">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11">
-        <f t="shared" ca="1" si="1"/>
-        <v>750</v>
+        <v>866</v>
       </c>
       <c r="C11">
         <v>473</v>
       </c>
       <c r="D11">
+        <v>0.34</v>
+      </c>
+      <c r="E11">
         <v>0.44</v>
       </c>
-      <c r="E11">
+      <c r="F11">
+        <v>281</v>
+      </c>
+      <c r="G11">
+        <v>0.23</v>
+      </c>
+      <c r="H11">
         <v>0.34</v>
       </c>
-      <c r="F11">
-        <v>0.41</v>
-      </c>
-      <c r="G11">
-        <v>0.31</v>
-      </c>
-      <c r="H11">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12">
-        <f t="shared" ca="1" si="1"/>
-        <v>894</v>
+        <v>736</v>
       </c>
       <c r="C12">
         <v>329</v>
       </c>
       <c r="D12">
+        <v>0.38</v>
+      </c>
+      <c r="E12">
         <v>0.43</v>
       </c>
-      <c r="E12">
+      <c r="F12">
+        <v>232</v>
+      </c>
+      <c r="G12">
+        <v>0.3</v>
+      </c>
+      <c r="H12">
         <v>0.38</v>
       </c>
-      <c r="F12">
-        <v>0.44</v>
-      </c>
-      <c r="G12">
-        <v>0.31</v>
-      </c>
-      <c r="H12">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13">
-        <f t="shared" ca="1" si="1"/>
-        <v>772</v>
+        <v>1000</v>
       </c>
       <c r="C13">
         <v>418</v>
       </c>
       <c r="D13">
+        <v>0.39</v>
+      </c>
+      <c r="E13">
         <v>0.41</v>
       </c>
-      <c r="E13">
+      <c r="F13">
+        <v>390</v>
+      </c>
+      <c r="G13">
+        <v>0.25</v>
+      </c>
+      <c r="H13">
         <v>0.39</v>
       </c>
-      <c r="F13">
-        <v>0.47</v>
-      </c>
-      <c r="G13">
-        <v>0.4</v>
-      </c>
-      <c r="H13">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14">
-        <f t="shared" ca="1" si="1"/>
-        <v>811</v>
+        <v>931</v>
       </c>
       <c r="C14">
         <v>496</v>
       </c>
       <c r="D14">
+        <v>0.33</v>
+      </c>
+      <c r="E14">
         <v>0.48</v>
       </c>
-      <c r="E14">
+      <c r="F14">
+        <v>883</v>
+      </c>
+      <c r="G14">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H14">
         <v>0.33</v>
       </c>
-      <c r="F14">
-        <v>0.42</v>
-      </c>
-      <c r="G14">
-        <v>0.34</v>
-      </c>
-      <c r="H14">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15">
-        <f t="shared" ca="1" si="1"/>
-        <v>801</v>
+        <v>791</v>
       </c>
       <c r="C15">
         <v>355</v>
       </c>
       <c r="D15">
+        <v>0.34</v>
+      </c>
+      <c r="E15">
         <v>0.49</v>
       </c>
-      <c r="E15">
+      <c r="F15">
+        <v>955</v>
+      </c>
+      <c r="G15">
+        <v>0.3</v>
+      </c>
+      <c r="H15">
         <v>0.34</v>
       </c>
-      <c r="F15">
-        <v>0.43</v>
-      </c>
-      <c r="G15">
-        <v>0.32</v>
-      </c>
-      <c r="H15">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16">
-        <f t="shared" ca="1" si="1"/>
-        <v>816</v>
+        <v>705</v>
       </c>
       <c r="C16">
         <v>327</v>
       </c>
       <c r="D16">
+        <v>0.32</v>
+      </c>
+      <c r="E16">
         <v>0.47</v>
       </c>
-      <c r="E16">
+      <c r="F16">
+        <v>841</v>
+      </c>
+      <c r="G16">
+        <v>0.21</v>
+      </c>
+      <c r="H16">
         <v>0.32</v>
-      </c>
-      <c r="F16">
-        <v>0.4</v>
-      </c>
-      <c r="G16">
-        <v>0.4</v>
-      </c>
-      <c r="H16">
-        <v>841</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1037,26 +1045,25 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <f t="shared" ca="1" si="1"/>
-        <v>758</v>
+        <v>820</v>
       </c>
       <c r="C17">
         <v>379</v>
       </c>
       <c r="D17">
+        <v>0.39</v>
+      </c>
+      <c r="E17">
         <v>0.48</v>
       </c>
-      <c r="E17">
+      <c r="F17">
+        <v>385</v>
+      </c>
+      <c r="G17">
+        <v>0.21</v>
+      </c>
+      <c r="H17">
         <v>0.39</v>
-      </c>
-      <c r="F17">
-        <v>0.43</v>
-      </c>
-      <c r="G17">
-        <v>0.32</v>
-      </c>
-      <c r="H17">
-        <v>385</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1065,26 +1072,25 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <f t="shared" ca="1" si="1"/>
-        <v>994</v>
+        <v>703</v>
       </c>
       <c r="C18">
         <v>440</v>
       </c>
       <c r="D18">
+        <v>0.33</v>
+      </c>
+      <c r="E18">
         <v>0.49</v>
       </c>
-      <c r="E18">
+      <c r="F18">
+        <v>672</v>
+      </c>
+      <c r="G18">
+        <v>0.26</v>
+      </c>
+      <c r="H18">
         <v>0.33</v>
-      </c>
-      <c r="F18">
-        <v>0.41</v>
-      </c>
-      <c r="G18">
-        <v>0.3</v>
-      </c>
-      <c r="H18">
-        <v>672</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1093,26 +1099,25 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <f t="shared" ca="1" si="1"/>
-        <v>945</v>
+        <v>841</v>
       </c>
       <c r="C19">
         <v>352</v>
       </c>
       <c r="D19">
+        <v>0.31</v>
+      </c>
+      <c r="E19">
         <v>0.5</v>
       </c>
-      <c r="E19">
+      <c r="F19">
+        <v>547</v>
+      </c>
+      <c r="G19">
+        <v>0.22</v>
+      </c>
+      <c r="H19">
         <v>0.31</v>
-      </c>
-      <c r="F19">
-        <v>0.48</v>
-      </c>
-      <c r="G19">
-        <v>0.36</v>
-      </c>
-      <c r="H19">
-        <v>547</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1121,26 +1126,25 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <f t="shared" ca="1" si="1"/>
-        <v>806</v>
+        <v>850</v>
       </c>
       <c r="C20">
         <v>381</v>
       </c>
       <c r="D20">
+        <v>0.32</v>
+      </c>
+      <c r="E20">
         <v>0.47</v>
       </c>
-      <c r="E20">
+      <c r="F20">
+        <v>552</v>
+      </c>
+      <c r="G20">
+        <v>0.27</v>
+      </c>
+      <c r="H20">
         <v>0.32</v>
-      </c>
-      <c r="F20">
-        <v>0.46</v>
-      </c>
-      <c r="G20">
-        <v>0.3</v>
-      </c>
-      <c r="H20">
-        <v>552</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1149,26 +1153,25 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <f t="shared" ca="1" si="1"/>
-        <v>838</v>
+        <v>798</v>
       </c>
       <c r="C21">
         <v>354</v>
       </c>
       <c r="D21">
+        <v>0.31</v>
+      </c>
+      <c r="E21">
         <v>0.4</v>
       </c>
-      <c r="E21">
+      <c r="F21">
+        <v>976</v>
+      </c>
+      <c r="G21">
+        <v>0.23</v>
+      </c>
+      <c r="H21">
         <v>0.31</v>
-      </c>
-      <c r="F21">
-        <v>0.46</v>
-      </c>
-      <c r="G21">
-        <v>0.31</v>
-      </c>
-      <c r="H21">
-        <v>976</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1177,26 +1180,25 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <f t="shared" ca="1" si="1"/>
-        <v>779</v>
+        <v>904</v>
       </c>
       <c r="C22">
         <v>440</v>
       </c>
       <c r="D22">
+        <v>0.3</v>
+      </c>
+      <c r="E22">
         <v>0.49</v>
       </c>
-      <c r="E22">
+      <c r="F22">
+        <v>734</v>
+      </c>
+      <c r="G22">
+        <v>0.25</v>
+      </c>
+      <c r="H22">
         <v>0.3</v>
-      </c>
-      <c r="F22">
-        <v>0.43</v>
-      </c>
-      <c r="G22">
-        <v>0.34</v>
-      </c>
-      <c r="H22">
-        <v>734</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1205,26 +1207,25 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <f t="shared" ca="1" si="1"/>
-        <v>898</v>
+        <v>767</v>
       </c>
       <c r="C23">
         <v>363</v>
       </c>
       <c r="D23">
+        <v>0.39</v>
+      </c>
+      <c r="E23">
         <v>0.41</v>
       </c>
-      <c r="E23">
+      <c r="F23">
+        <v>388</v>
+      </c>
+      <c r="G23">
+        <v>0.3</v>
+      </c>
+      <c r="H23">
         <v>0.39</v>
-      </c>
-      <c r="F23">
-        <v>0.47</v>
-      </c>
-      <c r="G23">
-        <v>0.39</v>
-      </c>
-      <c r="H23">
-        <v>388</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1233,26 +1234,25 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <f t="shared" ca="1" si="1"/>
-        <v>994</v>
+        <v>852</v>
       </c>
       <c r="C24">
         <v>397</v>
       </c>
       <c r="D24">
+        <v>0.4</v>
+      </c>
+      <c r="E24">
         <v>0.45</v>
       </c>
-      <c r="E24">
+      <c r="F24">
+        <v>731</v>
+      </c>
+      <c r="G24">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H24">
         <v>0.4</v>
-      </c>
-      <c r="F24">
-        <v>0.45</v>
-      </c>
-      <c r="G24">
-        <v>0.4</v>
-      </c>
-      <c r="H24">
-        <v>731</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1261,31 +1261,30 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <f t="shared" ca="1" si="1"/>
-        <v>739</v>
+        <v>749</v>
       </c>
       <c r="C25">
         <v>471</v>
       </c>
       <c r="D25">
+        <v>0.4</v>
+      </c>
+      <c r="E25">
         <v>0.45</v>
       </c>
-      <c r="E25">
+      <c r="F25">
+        <v>754</v>
+      </c>
+      <c r="G25">
+        <v>0.23</v>
+      </c>
+      <c r="H25">
         <v>0.4</v>
-      </c>
-      <c r="F25">
-        <v>0.49</v>
-      </c>
-      <c r="G25">
-        <v>0.36</v>
-      </c>
-      <c r="H25">
-        <v>754</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -1293,22 +1292,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1336,31 +1337,108 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="9.7890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.3125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E7" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E9" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="3" t="s">
-        <v>20</v>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1374,10 +1452,13 @@
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="3" t="s">
-        <v>21</v>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1391,10 +1472,13 @@
       <c r="E3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="3" t="s">
-        <v>22</v>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1408,10 +1492,13 @@
       <c r="E4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="3" t="s">
-        <v>23</v>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1423,6 +1510,97 @@
         <v>1</v>
       </c>
       <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
corrected problem calculating costs
</commit_message>
<xml_diff>
--- a/input/df_input.xlsx
+++ b/input/df_input.xlsx
@@ -8,17 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\02. Mestrado\TU Darmstadt\Energy Science and Engineering\5. Sommersemester 2023\Masterarbeit\5. Thesis\3. Python Routine\masterthesis\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015E7023-980E-43DF-B8AA-E6D21C2828A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8453155-2A51-46DB-AFE8-53AF0D5D128A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="other" sheetId="1" r:id="rId1"/>
     <sheet name="series" sheetId="2" r:id="rId2"/>
-    <sheet name="elements" sheetId="3" r:id="rId3"/>
-    <sheet name="elements test" sheetId="4" r:id="rId4"/>
-    <sheet name="conect_electric" sheetId="5" r:id="rId5"/>
-    <sheet name="conect_thermal" sheetId="6" r:id="rId6"/>
+    <sheet name="elements test" sheetId="3" r:id="rId3"/>
+    <sheet name="conect_electric" sheetId="4" r:id="rId4"/>
+    <sheet name="conect_thermal" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>Parameter</t>
   </si>
@@ -97,6 +96,12 @@
     <t>net1_cost_buy_thermal</t>
   </si>
   <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t># components</t>
+  </si>
+  <si>
     <t>demand</t>
   </si>
   <si>
@@ -107,12 +112,6 @@
   </si>
   <si>
     <t>bat</t>
-  </si>
-  <si>
-    <t>component</t>
-  </si>
-  <si>
-    <t># components</t>
   </si>
   <si>
     <t>CHP</t>
@@ -137,16 +136,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -164,6 +155,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -200,14 +192,13 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -593,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -655,7 +646,7 @@
         <v>893</v>
       </c>
       <c r="G2">
-        <v>0.23</v>
+        <v>0.16</v>
       </c>
       <c r="H2">
         <v>0.4</v>
@@ -682,7 +673,7 @@
         <v>632</v>
       </c>
       <c r="G3">
-        <v>0.25</v>
+        <v>0.12</v>
       </c>
       <c r="H3">
         <v>0.38</v>
@@ -709,7 +700,7 @@
         <v>212</v>
       </c>
       <c r="G4">
-        <v>0.24</v>
+        <v>0.19</v>
       </c>
       <c r="H4">
         <v>0.3</v>
@@ -736,7 +727,7 @@
         <v>580</v>
       </c>
       <c r="G5">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="H5">
         <v>0.34</v>
@@ -763,7 +754,7 @@
         <v>607</v>
       </c>
       <c r="G6">
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="H6">
         <v>0.31</v>
@@ -790,7 +781,7 @@
         <v>177</v>
       </c>
       <c r="G7">
-        <v>0.22</v>
+        <v>0.18</v>
       </c>
       <c r="H7">
         <v>0.36</v>
@@ -817,7 +808,7 @@
         <v>735</v>
       </c>
       <c r="G8">
-        <v>0.27</v>
+        <v>0.1</v>
       </c>
       <c r="H8">
         <v>0.38</v>
@@ -844,7 +835,7 @@
         <v>879</v>
       </c>
       <c r="G9">
-        <v>0.27</v>
+        <v>0.19</v>
       </c>
       <c r="H9">
         <v>0.39</v>
@@ -871,7 +862,7 @@
         <v>731</v>
       </c>
       <c r="G10">
-        <v>0.3</v>
+        <v>0.19</v>
       </c>
       <c r="H10">
         <v>0.35</v>
@@ -898,7 +889,7 @@
         <v>281</v>
       </c>
       <c r="G11">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="H11">
         <v>0.34</v>
@@ -925,7 +916,7 @@
         <v>232</v>
       </c>
       <c r="G12">
-        <v>0.3</v>
+        <v>0.13</v>
       </c>
       <c r="H12">
         <v>0.38</v>
@@ -952,7 +943,7 @@
         <v>390</v>
       </c>
       <c r="G13">
-        <v>0.25</v>
+        <v>0.18</v>
       </c>
       <c r="H13">
         <v>0.39</v>
@@ -979,7 +970,7 @@
         <v>883</v>
       </c>
       <c r="G14">
-        <v>0.28999999999999998</v>
+        <v>0.16</v>
       </c>
       <c r="H14">
         <v>0.33</v>
@@ -1006,7 +997,7 @@
         <v>955</v>
       </c>
       <c r="G15">
-        <v>0.3</v>
+        <v>0.12</v>
       </c>
       <c r="H15">
         <v>0.34</v>
@@ -1033,7 +1024,7 @@
         <v>841</v>
       </c>
       <c r="G16">
-        <v>0.21</v>
+        <v>0.1</v>
       </c>
       <c r="H16">
         <v>0.32</v>
@@ -1060,7 +1051,7 @@
         <v>385</v>
       </c>
       <c r="G17">
-        <v>0.21</v>
+        <v>0.17</v>
       </c>
       <c r="H17">
         <v>0.39</v>
@@ -1087,7 +1078,7 @@
         <v>672</v>
       </c>
       <c r="G18">
-        <v>0.26</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H18">
         <v>0.33</v>
@@ -1114,7 +1105,7 @@
         <v>547</v>
       </c>
       <c r="G19">
-        <v>0.22</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H19">
         <v>0.31</v>
@@ -1141,7 +1132,7 @@
         <v>552</v>
       </c>
       <c r="G20">
-        <v>0.27</v>
+        <v>0.13</v>
       </c>
       <c r="H20">
         <v>0.32</v>
@@ -1168,7 +1159,7 @@
         <v>976</v>
       </c>
       <c r="G21">
-        <v>0.23</v>
+        <v>0.19</v>
       </c>
       <c r="H21">
         <v>0.31</v>
@@ -1195,7 +1186,7 @@
         <v>734</v>
       </c>
       <c r="G22">
-        <v>0.25</v>
+        <v>0.13</v>
       </c>
       <c r="H22">
         <v>0.3</v>
@@ -1222,7 +1213,7 @@
         <v>388</v>
       </c>
       <c r="G23">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="H23">
         <v>0.39</v>
@@ -1249,7 +1240,7 @@
         <v>731</v>
       </c>
       <c r="G24">
-        <v>0.28999999999999998</v>
+        <v>0.19</v>
       </c>
       <c r="H24">
         <v>0.4</v>
@@ -1276,7 +1267,7 @@
         <v>754</v>
       </c>
       <c r="G25">
-        <v>0.23</v>
+        <v>0.19</v>
       </c>
       <c r="H25">
         <v>0.4</v>
@@ -1284,63 +1275,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E4" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1351,15 +1295,15 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1367,7 +1311,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1375,7 +1319,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1383,7 +1327,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1398,10 +1342,10 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E7" s="2"/>
+      <c r="E7" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E9" s="3"/>
+      <c r="E9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1409,35 +1353,35 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B2">
@@ -1457,7 +1401,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B3">
@@ -1477,7 +1421,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B4">
@@ -1497,7 +1441,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B5">
@@ -1517,7 +1461,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B6">
@@ -1541,29 +1485,29 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B2">
@@ -1577,7 +1521,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B3">
@@ -1591,7 +1535,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B4">

</xml_diff>